<commit_message>
Actulizacion del diagrama de flujo
</commit_message>
<xml_diff>
--- a/src/Respuestas_Form.xlsx
+++ b/src/Respuestas_Form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lauren\Documentos\Cursos Online\Programacion\Talento Tech\Proyecto Final\www.chinchin.com\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A703F8DD-0370-461B-ACB5-E8B714AF8FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191CB1B6-69AF-4B06-948F-9282D212EAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1088,9 +1087,9 @@
   </sheetPr>
   <dimension ref="A1:AC51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA1" sqref="AA1"/>
+      <selection pane="bottomLeft" activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>